<commit_message>
Keywords SEO + hover Dark/Light
</commit_message>
<xml_diff>
--- a/reports/SEO_ANALYSE_RECO_20200309.xlsx
+++ b/reports/SEO_ANALYSE_RECO_20200309.xlsx
@@ -5,25 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Famille\Alexandre\FORMATIONS\DEV\PROJETS\04_PROJET_OPTIMISER_SITE_WEB\PROJET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\p4\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE71A11D-FE15-472B-BE19-97FB8ADFFC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679E08F3-A24A-48D3-A9D5-B26B3B3DE509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse SEO + RECO" sheetId="1" r:id="rId1"/>
+    <sheet name="keywords" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Analyse SEO + RECO'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">keywords!$A$1:$A$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>Categorie</t>
   </si>
@@ -230,13 +232,73 @@
   </si>
   <si>
     <t>Structure hiérarchique</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Web Design</t>
+  </si>
+  <si>
+    <t>Agence Web</t>
+  </si>
+  <si>
+    <t>Agence Web Design</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Design thinking</t>
+  </si>
+  <si>
+    <t>Mobile first</t>
+  </si>
+  <si>
+    <t>Conception graphique</t>
+  </si>
+  <si>
+    <t>Positionnement graphique</t>
+  </si>
+  <si>
+    <t>Univers coloriel</t>
+  </si>
+  <si>
+    <t>Ergonomie</t>
+  </si>
+  <si>
+    <t>Evolutions technologiques</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Responsive</t>
+  </si>
+  <si>
+    <t>Logotype</t>
+  </si>
+  <si>
+    <t>Charte graphique</t>
+  </si>
+  <si>
+    <t>Identité visuelle</t>
+  </si>
+  <si>
+    <t>Design fonctionnel</t>
+  </si>
+  <si>
+    <t>Design Emotionnel</t>
+  </si>
+  <si>
+    <t>UX/UI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,8 +361,51 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFCC0066"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF047DB0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +416,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF047DB0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF047DB0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -334,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -374,6 +485,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -384,9 +501,9 @@
   <colors>
     <mruColors>
       <color rgb="FF047DB0"/>
+      <color rgb="FFCC0066"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FFCC0066"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1399,4 +1516,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId16"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05470FC6-6D4A-4146-93D8-3818643944A6}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.5546875" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A5" xr:uid="{28308445-A3C8-4750-935B-EC05770AF183}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ppt & reports updated
</commit_message>
<xml_diff>
--- a/reports/SEO_ANALYSE_RECO_20200309.xlsx
+++ b/reports/SEO_ANALYSE_RECO_20200309.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\p4\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AB35B7-F71A-4442-BB77-785602608DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB103B9-9B46-4D3F-B115-460DCDDD7729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse SEO + RECO" sheetId="1" r:id="rId1"/>
@@ -731,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1536,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05470FC6-6D4A-4146-93D8-3818643944A6}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>